<commit_message>
Updated version of the World Description Document
</commit_message>
<xml_diff>
--- a/Project Documents/World Description.xlsx
+++ b/Project Documents/World Description.xlsx
@@ -24,23 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>Describe Role in game</t>
   </si>
   <si>
-    <t>Text description of role in game</t>
-  </si>
-  <si>
     <t>Internal Functionality</t>
   </si>
   <si>
     <t>Text Description</t>
   </si>
   <si>
-    <t>Eg Turn Left</t>
-  </si>
-  <si>
     <t>External Outgoing</t>
   </si>
   <si>
@@ -50,18 +44,12 @@
     <t>Communication with?</t>
   </si>
   <si>
-    <t>Eg Push</t>
-  </si>
-  <si>
     <t>External Incoming</t>
   </si>
   <si>
     <t xml:space="preserve">Return </t>
   </si>
   <si>
-    <t>ShouldTurnLeft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
@@ -72,15 +60,130 @@
   </si>
   <si>
     <t>Item Name (Jack)</t>
+  </si>
+  <si>
+    <t>Ice Blocks</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Instantiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Communicate with the ice blocks to set up the starting positions of the ice blocks as well as display the size and dimensions of the cubes across random positions in the game area.</t>
+  </si>
+  <si>
+    <t>Enemies</t>
+  </si>
+  <si>
+    <t>EnemyUnderTile</t>
+  </si>
+  <si>
+    <t>EnemyInLineOfIceBlock</t>
+  </si>
+  <si>
+    <t>Enemies/Ice Blocks</t>
+  </si>
+  <si>
+    <t>Determines if enemy is in place to be smashed by an ice block.</t>
+  </si>
+  <si>
+    <t>Creating Enemies</t>
+  </si>
+  <si>
+    <t>ScoreShowingUp</t>
+  </si>
+  <si>
+    <t>Spawn the egg and enemy</t>
+  </si>
+  <si>
+    <t>Forms a new enemy (Spawn from an egg) and decides the spawning of the enemies in random positions.</t>
+  </si>
+  <si>
+    <t>The world is in charge of most game components which will determine most of the game. It is in charge of the ice block's position,size and dimension. It is also responsible for communicating with the enemies,the egg and the pop-up score to  and decide the game's progression.</t>
+  </si>
+  <si>
+    <t>The world controls the collision clause when the player pushes the ice block.</t>
+  </si>
+  <si>
+    <t>Commands Scripts</t>
+  </si>
+  <si>
+    <t>Develop the level area required for the game by forming the floor for the penguin to move and the walls blocking the area.</t>
+  </si>
+  <si>
+    <t>Create the world area</t>
+  </si>
+  <si>
+    <t>It provides the basis for combining the codes together as they can all communicate with the world to control the game mechanics and to ensure that the game runs smoothly.</t>
+  </si>
+  <si>
+    <t>The world must allow the ice blocks to move when it detects the movement of the ice blocks when pushed. It will require a particular distance for the block to be pushed.</t>
+  </si>
+  <si>
+    <t>Communicates with the enemy script when the enemy is killed by the player and is put under a particular tile where it's placed.</t>
+  </si>
+  <si>
+    <t>Allows the creation of a new enemy (Spawn from new egg) and in charge of position of egg.</t>
+  </si>
+  <si>
+    <t>Distance/Integer</t>
+  </si>
+  <si>
+    <t>Detect Movement when pushed</t>
+  </si>
+  <si>
+    <t>Allows for the cloning of the ice blocks where the world stores the method script for instantiation so they can have the same design when it's displayed in the game world's area.</t>
+  </si>
+  <si>
+    <t>Set up the Ice Blocks</t>
+  </si>
+  <si>
+    <t>Ice Blocks/Rocks/Game Manager</t>
+  </si>
+  <si>
+    <t>Enables a change in the score that pops up for a brief time when the penguin gets fruit and money as the world communicates with the score through the game manager..</t>
+  </si>
+  <si>
+    <t>Pop Up Score/Game Manager</t>
+  </si>
+  <si>
+    <t>Enemies/Egg/Game Manager</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,9 +210,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,118 +503,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="2" width="255.42578125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
+    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final Version of the World Description Document
</commit_message>
<xml_diff>
--- a/Project Documents/World Description.xlsx
+++ b/Project Documents/World Description.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00194492\Desktop\Push-Penguin3D\Project Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Yr 2 Semester 1\Games Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,23 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Describe Role in game</t>
   </si>
   <si>
-    <t>Text description of role in game</t>
-  </si>
-  <si>
     <t>Internal Functionality</t>
   </si>
   <si>
     <t>Text Description</t>
   </si>
   <si>
-    <t>Eg Turn Left</t>
-  </si>
-  <si>
     <t>External Outgoing</t>
   </si>
   <si>
@@ -50,18 +44,12 @@
     <t>Communication with?</t>
   </si>
   <si>
-    <t>Eg Push</t>
-  </si>
-  <si>
     <t>External Incoming</t>
   </si>
   <si>
     <t xml:space="preserve">Return </t>
   </si>
   <si>
-    <t>ShouldTurnLeft</t>
-  </si>
-  <si>
     <t xml:space="preserve">Name of InterFace </t>
   </si>
   <si>
@@ -72,15 +60,142 @@
   </si>
   <si>
     <t>Item Name (Jack)</t>
+  </si>
+  <si>
+    <t>Ice Blocks</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Instantiation</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Communicate with the ice blocks to set up the starting positions of the ice blocks as well as display the size and dimensions of the cubes across random positions in the game area.</t>
+  </si>
+  <si>
+    <t>Enemies</t>
+  </si>
+  <si>
+    <t>EnemyUnderTile</t>
+  </si>
+  <si>
+    <t>EnemyInLineOfIceBlock</t>
+  </si>
+  <si>
+    <t>Enemies/Ice Blocks</t>
+  </si>
+  <si>
+    <t>Determines if enemy is in place to be smashed by an ice block.</t>
+  </si>
+  <si>
+    <t>Creating Enemies</t>
+  </si>
+  <si>
+    <t>ScoreShowingUp</t>
+  </si>
+  <si>
+    <t>Spawn the egg and enemy</t>
+  </si>
+  <si>
+    <t>Forms a new enemy (Spawn from an egg) and decides the spawning of the enemies in random positions.</t>
+  </si>
+  <si>
+    <t>The world is in charge of most game components which will determine most of the game. It is in charge of the ice block's position,size and dimension. It is also responsible for communicating with the enemies,the egg and the pop-up score to  and decide the game's progression.</t>
+  </si>
+  <si>
+    <t>The world controls the collision clause when the player pushes the ice block.</t>
+  </si>
+  <si>
+    <t>Commands Scripts</t>
+  </si>
+  <si>
+    <t>Develop the level area required for the game by forming the floor for the penguin to move and the walls blocking the area.</t>
+  </si>
+  <si>
+    <t>Create the world area</t>
+  </si>
+  <si>
+    <t>It provides the basis for combining the codes together as they can all communicate with the world to control the game mechanics and to ensure that the game runs smoothly.</t>
+  </si>
+  <si>
+    <t>The world must allow the ice blocks to move when it detects the movement of the ice blocks when pushed. It will require a particular distance for the block to be pushed.</t>
+  </si>
+  <si>
+    <t>Communicates with the enemy script when the enemy is killed by the player and is put under a particular tile where it's placed.</t>
+  </si>
+  <si>
+    <t>Allows the creation of a new enemy (Spawn from new egg) and in charge of position of egg.</t>
+  </si>
+  <si>
+    <t>Distance/Integer</t>
+  </si>
+  <si>
+    <t>Detect Movement when pushed</t>
+  </si>
+  <si>
+    <t>Allows for the cloning of the ice blocks where the world stores the method script for instantiation so they can have the same design when it's displayed in the game world's area.</t>
+  </si>
+  <si>
+    <t>Set up the Ice Blocks</t>
+  </si>
+  <si>
+    <t>Ice Blocks/Rocks/Game Manager</t>
+  </si>
+  <si>
+    <t>Enables a change in the score that pops up for a brief time when the penguin gets fruit and money as the world communicates with the score through the game manager..</t>
+  </si>
+  <si>
+    <t>Pop Up Score/Game Manager</t>
+  </si>
+  <si>
+    <t>Enemies/Egg/Game Manager</t>
+  </si>
+  <si>
+    <t>Death/HP</t>
+  </si>
+  <si>
+    <t>Penguin/Enemies</t>
+  </si>
+  <si>
+    <t>Damage/Destruction of Penguin</t>
+  </si>
+  <si>
+    <t>Indicates whether the enemy will be destroyed or lose health depending on the damage inflicted by the enemy.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -107,9 +222,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,118 +515,323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="41.7109375" customWidth="1"/>
+    <col min="2" max="2" width="255.42578125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" customWidth="1"/>
+    <col min="6" max="6" width="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>15</v>
+    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="3" spans="1:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>9</v>
+    </row>
+    <row r="11" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>10</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>13</v>
-      </c>
+    </row>
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>